<commit_message>
Move regression estimates to country specific folder
</commit_message>
<xml_diff>
--- a/input/DatabaseCountryYear.xlsx
+++ b/input/DatabaseCountryYear.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\labsim\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPathsEU\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D815BC53-4306-44EF-9B0C-88D2EAD4BB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C05C72E-AA08-411D-9D66-8A67D7D3EC70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{76CA3BB5-FA62-4FEC-A3AF-26EB81C6ADDD}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Country</t>
   </si>
@@ -41,35 +41,16 @@
     <t>Year</t>
   </si>
   <si>
-    <t>UK</t>
-  </si>
-  <si>
-    <t>2011</t>
-  </si>
-  <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>2017</t>
-  </si>
-  <si>
-    <t>2012</t>
-  </si>
-  <si>
     <t>2019</t>
   </si>
   <si>
-    <t>HU</t>
-  </si>
-  <si>
-    <t>PL</t>
+    <t>EL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -119,9 +100,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -159,7 +140,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -265,7 +246,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -407,7 +388,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -421,7 +402,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,12 +410,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>